<commit_message>
Added SF GI data and visualization
</commit_message>
<xml_diff>
--- a/BR_designstorm_data.xlsx
+++ b/BR_designstorm_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/BMPPerformanceIndexLACounty-AdvisoryCommittee/Shared Documents/Advisory Committee/Framework Development/Eddie Investigation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_334B89138F8D492AC4F4F5572E7E105D2F3828CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_334B89138F8D492AC4F4F5572E7E105D2F3828CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{729465D8-ACBD-486B-9E75-9612A28E9586}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,8 @@
   <dimension ref="A1:N456"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <pane ySplit="1" topLeftCell="A441" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H465" sqref="H465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20570,15 +20571,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044F1BAFAFA5C994385C29346B356BB10" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ce5f4bc358c2b9860ee5483fa7530a4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4850582b-7731-4c40-8c55-dde852aa0ecb" xmlns:ns3="4a324a06-9923-4017-aacf-b7275f71a724" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7039789a7397ee55336f130558b4def6" ns2:_="" ns3:_="">
     <xsd:import namespace="4850582b-7731-4c40-8c55-dde852aa0ecb"/>
@@ -20809,15 +20801,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D5FD2C4-D405-4D16-A4D3-2C64CC92B65B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EBFC889-CB4E-4C2F-904F-BAAC34D0D88F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20834,4 +20827,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D5FD2C4-D405-4D16-A4D3-2C64CC92B65B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>